<commit_message>
Calibrated the campus centre map
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2081B69-1011-4F19-93E8-54E29694DB15}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA32287-F81C-44A3-9BCA-B4783A6F11A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{545FE80B-02C6-4C0D-8784-416F53C454F8}"/>
   </bookViews>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5722D427-E56D-4A4D-A099-7E5EFC806B94}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
finished allocation.py and industries are now dynamic
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HansingJ\Desktop\Swapstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Swapstone\Excel Testing\BlackBoard Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF0F4F7-5C71-4052-9450-C71CD4C7CD84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5405EA2-8379-459B-BEDD-4AA857BBC7AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{545FE80B-02C6-4C0D-8784-416F53C454F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{545FE80B-02C6-4C0D-8784-416F53C454F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -606,17 +606,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5722D427-E56D-4A4D-A099-7E5EFC806B94}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="6" max="6" width="20.54296875" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -636,7 +636,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -656,7 +656,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -676,7 +676,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -696,7 +696,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -716,7 +716,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -736,7 +736,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -756,7 +756,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -776,7 +776,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -796,7 +796,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -816,7 +816,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -836,7 +836,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -856,7 +856,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -876,7 +876,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -896,7 +896,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -916,7 +916,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -936,7 +936,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -956,7 +956,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -976,7 +976,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -996,7 +996,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>

</xml_diff>